<commit_message>
Added rml_modules_injector CLI command
</commit_message>
<xml_diff>
--- a/tests/test_data/notice_transformer/mapping_suite_processor_repository/test_package/transformation/conceptual_mappings.xlsx
+++ b/tests/test_data/notice_transformer/mapping_suite_processor_repository/test_package/transformation/conceptual_mappings.xlsx
@@ -5,24 +5,25 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Rules" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Resources" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Legend" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Ex sample data" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Ex Controlled List of Roles (CL" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Ex Controlled List for Organisa" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="CL3 (at-vocnuts)" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="CL4 (at-voccountry)" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="CL5 (at-vocbuyer-legal-type)" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="CL6 (at-vocmain-activity)" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="CL7 (at-voccpv)" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="CL8 (at-voccontract-nature)" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="CL9 (at-voccurrency)" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Questions" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="RML_Modules" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Legend" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Ex sample data" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Ex Controlled List of Roles (CL" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Ex Controlled List for Organisa" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="CL3 (at-vocnuts)" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="CL4 (at-voccountry)" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="CL5 (at-vocbuyer-legal-type)" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="CL6 (at-vocmain-activity)" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="CL7 (at-voccpv)" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="CL8 (at-voccontract-nature)" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="CL9 (at-voccurrency)" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Questions" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -383,7 +384,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="725">
   <si>
     <t xml:space="preserve">Field</t>
   </si>
@@ -4218,6 +4219,45 @@
   </si>
   <si>
     <t xml:space="preserve">nuts.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment (optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">technical_mapping_F03.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first file listed should always be the main file (i.e. the "entry point" specific to a form)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contracting_authority.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">section 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">section 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procedure.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">section 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">award_of_contract.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">section 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complementary_information.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">section 6</t>
   </si>
   <si>
     <t xml:space="preserve">Property path</t>
@@ -4386,7 +4426,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4472,6 +4512,21 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -4613,7 +4668,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4814,6 +4869,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4866,7 +4929,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4986,11 +5049,11 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="26.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5157,24 +5220,24 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>
@@ -5202,24 +5265,24 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>
@@ -5247,24 +5310,24 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>
@@ -5292,24 +5355,24 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>
@@ -5337,24 +5400,24 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>
@@ -5376,13 +5439,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -5411,7 +5519,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.22"/>
@@ -14336,7 +14444,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.22"/>
   </cols>
@@ -14372,100 +14480,183 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="50" t="s">
+        <v>673</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="51" t="s">
+        <v>677</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="51" t="s">
+        <v>679</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="51" t="s">
+        <v>681</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="51" t="s">
+        <v>683</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="51" t="s">
+        <v>685</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="51" t="s">
+        <v>687</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>688</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.78"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="50" t="s">
-        <v>676</v>
+      <c r="A2" s="52" t="s">
+        <v>689</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>677</v>
+        <v>690</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
-        <v>678</v>
+      <c r="A3" s="53" t="s">
+        <v>691</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>679</v>
+        <v>692</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="52" t="s">
-        <v>680</v>
+      <c r="A4" s="54" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="53" t="s">
-        <v>681</v>
+      <c r="A8" s="55" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="53" t="s">
-        <v>682</v>
+      <c r="A9" s="55" t="s">
+        <v>695</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>683</v>
+        <v>696</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="54" t="s">
-        <v>684</v>
+      <c r="B10" s="56" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
-      <c r="B11" s="55" t="s">
-        <v>685</v>
+      <c r="B11" s="57" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="56" t="s">
-        <v>686</v>
+      <c r="B12" s="58" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="57" t="s">
-        <v>687</v>
+      <c r="B13" s="59" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="58" t="s">
-        <v>688</v>
+      <c r="B14" s="60" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="53"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="53" t="s">
-        <v>689</v>
+      <c r="A16" s="55" t="s">
+        <v>702</v>
       </c>
       <c r="B16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="59"/>
+      <c r="B17" s="61"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="53" t="s">
-        <v>690</v>
+      <c r="A20" s="55" t="s">
+        <v>703</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>691</v>
+        <v>704</v>
       </c>
     </row>
   </sheetData>
@@ -14479,7 +14670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -14490,7 +14681,7 @@
       <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.66"/>
@@ -14591,35 +14782,35 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="60" t="s">
-        <v>692</v>
-      </c>
-      <c r="E5" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="F5" s="61" t="s">
-        <v>694</v>
-      </c>
-      <c r="G5" s="61" t="s">
-        <v>695</v>
-      </c>
-      <c r="H5" s="62" t="s">
-        <v>696</v>
-      </c>
-      <c r="I5" s="60" t="s">
-        <v>697</v>
-      </c>
-      <c r="J5" s="61" t="s">
-        <v>698</v>
+      <c r="D5" s="62" t="s">
+        <v>705</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>706</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>707</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>708</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>709</v>
+      </c>
+      <c r="I5" s="62" t="s">
+        <v>710</v>
+      </c>
+      <c r="J5" s="63" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14641,7 +14832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -14652,109 +14843,48 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>704</v>
+        <v>717</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>705</v>
+        <v>718</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>706</v>
+        <v>719</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>707</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>708</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>710</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>711</v>
+        <v>720</v>
       </c>
     </row>
   </sheetData>
@@ -14776,30 +14906,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>721</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>723</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>724</v>
       </c>
     </row>
   </sheetData>
@@ -14827,24 +14973,24 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="B1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>700</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>701</v>
+      <c r="A2" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CM reader & CM differ
</commit_message>
<xml_diff>
--- a/tests/test_data/notice_transformer/mapping_suite_processor_repository/test_package/transformation/conceptual_mappings.xlsx
+++ b/tests/test_data/notice_transformer/mapping_suite_processor_repository/test_package/transformation/conceptual_mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -4656,10 +4656,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -5229,7 +5230,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5410,7 +5411,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5587,7 +5588,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5656,7 +5657,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5717,7 +5718,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5762,7 +5763,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5807,7 +5808,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5852,7 +5853,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5897,7 +5898,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5942,7 +5943,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5987,7 +5988,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6032,7 +6033,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6061,7 +6062,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15249,18 +15250,18 @@
   </sheetPr>
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="35.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="40"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="7" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16470,7 +16471,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16512,7 +16513,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16595,7 +16596,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16746,8 +16747,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16833,7 +16834,7 @@
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16945,7 +16946,7 @@
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>